<commit_message>
Added sheet2 with graph
</commit_message>
<xml_diff>
--- a/WestBank-Hotels.xlsx
+++ b/WestBank-Hotels.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="7272"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="7272" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>السنة</t>
   </si>
@@ -64,6 +65,9 @@
   </si>
   <si>
     <t>Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.pcbs.gov.ps/Portals/_Rainbow/Documents/T.S-%20Tourism-%20An-A-2015.htm</t>
   </si>
 </sst>
 </file>
@@ -192,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
@@ -271,6 +275,13 @@
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,6 +298,514 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.5365664172999844E-2"/>
+          <c:y val="2.8252405949256341E-2"/>
+          <c:w val="0.90335220720741305"/>
+          <c:h val="0.7991849211976465"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>متوسط الإشغال السنوي لكل 200 سرير</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$L$3:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>30.642610186733165</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.537517237542275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.8391024045719</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.515907722891129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.11836867235138</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2749979493068668</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.969464443391673</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.8964423042595326</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7877969901434039</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.965746998547701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.597841966752263</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.079792833910972</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32.866142171550713</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30.658020065806419</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35.264882780455032</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.882214562809811</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.822436564725248</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>29.879035131113131</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28.517915626678242</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>25.83926055232979</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>نسبة إشغال الغرف %</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$3:$J$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>36.49707803368856</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.044359949302919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.808314087759815</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.717032967032964</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.219878105954052</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0404845393688245</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9222614840989412</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.932158297306286</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.551580964548068</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.480274442538594</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.235011990407671</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.475207719110156</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36.697530864197532</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34.851555136663521</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.919389978213509</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28.393107593668603</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.092831059004421</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.762308998302206</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25.231023102310235</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22.537181563834487</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="59704832"/>
+        <c:axId val="1208256"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="59704832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1208256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1208256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59704832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.222609981129408"/>
+          <c:y val="4.71976401179941E-2"/>
+          <c:w val="0.4090604453131883"/>
+          <c:h val="7.3990894943441798E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="1"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>251460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -578,7 +1097,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -598,25 +1117,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
       <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1611,4 +2130,1038 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="8.88671875" style="8"/>
+    <col min="9" max="9" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+    </row>
+    <row r="2" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A3" s="29">
+        <v>1996</v>
+      </c>
+      <c r="B3" s="4">
+        <v>65</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2909</v>
+      </c>
+      <c r="D3" s="5">
+        <v>6383</v>
+      </c>
+      <c r="E3" s="5">
+        <v>223322</v>
+      </c>
+      <c r="F3" s="5">
+        <v>713910</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1061.7</v>
+      </c>
+      <c r="H3" s="10">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="I3" s="9">
+        <f>(E3/(D3*365))*100</f>
+        <v>9.5854785506879363</v>
+      </c>
+      <c r="J3" s="36">
+        <f>(G3/C3)*100</f>
+        <v>36.49707803368856</v>
+      </c>
+      <c r="K3" s="9">
+        <f>F3/E3</f>
+        <v>3.1967741646591019</v>
+      </c>
+      <c r="L3" s="31">
+        <f>I3*K3</f>
+        <v>30.642610186733165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A4" s="29">
+        <v>1997</v>
+      </c>
+      <c r="B4" s="1">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3156</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6894</v>
+      </c>
+      <c r="E4" s="2">
+        <v>213933</v>
+      </c>
+      <c r="F4" s="2">
+        <v>617440</v>
+      </c>
+      <c r="G4" s="1">
+        <v>948.2</v>
+      </c>
+      <c r="H4" s="10">
+        <v>31.7</v>
+      </c>
+      <c r="I4" s="9">
+        <f>(E4/(D4*365))*100</f>
+        <v>8.501853905122978</v>
+      </c>
+      <c r="J4" s="36">
+        <f t="shared" ref="J4:J22" si="0">(G4/C4)*100</f>
+        <v>30.044359949302919</v>
+      </c>
+      <c r="K4" s="9">
+        <f>F4/E4</f>
+        <v>2.8861372485778256</v>
+      </c>
+      <c r="L4" s="31">
+        <f>I4*K4</f>
+        <v>24.537517237542275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A5" s="29">
+        <v>1998</v>
+      </c>
+      <c r="B5" s="4">
+        <v>83</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3464</v>
+      </c>
+      <c r="D5" s="5">
+        <v>7541</v>
+      </c>
+      <c r="E5" s="5">
+        <v>203852</v>
+      </c>
+      <c r="F5" s="5">
+        <v>573589</v>
+      </c>
+      <c r="G5" s="4">
+        <v>894</v>
+      </c>
+      <c r="H5" s="10">
+        <v>27.5</v>
+      </c>
+      <c r="I5" s="9">
+        <f>(E5/(D5*365))*100</f>
+        <v>7.4061613862483267</v>
+      </c>
+      <c r="J5" s="36">
+        <f t="shared" si="0"/>
+        <v>25.808314087759815</v>
+      </c>
+      <c r="K5" s="9">
+        <f>F5/E5</f>
+        <v>2.8137521339010654</v>
+      </c>
+      <c r="L5" s="31">
+        <f>I5*K5</f>
+        <v>20.8391024045719</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A6" s="29">
+        <v>1999</v>
+      </c>
+      <c r="B6" s="1">
+        <v>80</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3640</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7897</v>
+      </c>
+      <c r="E6" s="2">
+        <v>311114</v>
+      </c>
+      <c r="F6" s="2">
+        <v>850768</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1227.3</v>
+      </c>
+      <c r="H6" s="10">
+        <v>35.5</v>
+      </c>
+      <c r="I6" s="9">
+        <f>(E6/(D6*365))*100</f>
+        <v>10.793556075568839</v>
+      </c>
+      <c r="J6" s="36">
+        <f t="shared" si="0"/>
+        <v>33.717032967032964</v>
+      </c>
+      <c r="K6" s="9">
+        <f>F6/E6</f>
+        <v>2.7345860359868088</v>
+      </c>
+      <c r="L6" s="31">
+        <f>I6*K6</f>
+        <v>29.515907722891129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A7" s="29">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="4">
+        <v>94</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4266</v>
+      </c>
+      <c r="D7" s="5">
+        <v>9112</v>
+      </c>
+      <c r="E7" s="5">
+        <v>315709</v>
+      </c>
+      <c r="F7" s="5">
+        <v>968442</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1374.5</v>
+      </c>
+      <c r="H7" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="I7" s="9">
+        <f>(E7/(D7*365))*100</f>
+        <v>9.4924952193103778</v>
+      </c>
+      <c r="J7" s="36">
+        <f t="shared" si="0"/>
+        <v>32.219878105954052</v>
+      </c>
+      <c r="K7" s="9">
+        <f>F7/E7</f>
+        <v>3.0675147049973237</v>
+      </c>
+      <c r="L7" s="31">
+        <f>I7*K7</f>
+        <v>29.11836867235138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A8" s="29">
+        <v>2001</v>
+      </c>
+      <c r="B8" s="1">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3137</v>
+      </c>
+      <c r="D8" s="2">
+        <v>6680</v>
+      </c>
+      <c r="E8" s="2">
+        <v>57968</v>
+      </c>
+      <c r="F8" s="2">
+        <v>177379</v>
+      </c>
+      <c r="G8" s="1">
+        <v>283.60000000000002</v>
+      </c>
+      <c r="H8" s="10">
+        <v>8.4</v>
+      </c>
+      <c r="I8" s="9">
+        <f>(E8/(D8*365))*100</f>
+        <v>2.3774915921581496</v>
+      </c>
+      <c r="J8" s="36">
+        <f t="shared" si="0"/>
+        <v>9.0404845393688245</v>
+      </c>
+      <c r="K8" s="9">
+        <f>F8/E8</f>
+        <v>3.0599468672370964</v>
+      </c>
+      <c r="L8" s="31">
+        <f>I8*K8</f>
+        <v>7.2749979493068668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A9" s="29">
+        <v>2002</v>
+      </c>
+      <c r="B9" s="4">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2830</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6159</v>
+      </c>
+      <c r="E9" s="5">
+        <v>45239</v>
+      </c>
+      <c r="F9" s="5">
+        <v>156676</v>
+      </c>
+      <c r="G9" s="4">
+        <v>280.8</v>
+      </c>
+      <c r="H9" s="10">
+        <v>11.3</v>
+      </c>
+      <c r="I9" s="9">
+        <f>(E9/(D9*365))*100</f>
+        <v>2.012379700493987</v>
+      </c>
+      <c r="J9" s="36">
+        <f t="shared" si="0"/>
+        <v>9.9222614840989412</v>
+      </c>
+      <c r="K9" s="9">
+        <f>F9/E9</f>
+        <v>3.4632949446274233</v>
+      </c>
+      <c r="L9" s="31">
+        <f>I9*K9</f>
+        <v>6.969464443391673</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A10" s="29">
+        <v>2003</v>
+      </c>
+      <c r="B10" s="1">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3007</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6523</v>
+      </c>
+      <c r="E10" s="2">
+        <v>58256</v>
+      </c>
+      <c r="F10" s="2">
+        <v>188006</v>
+      </c>
+      <c r="G10" s="1">
+        <v>358.8</v>
+      </c>
+      <c r="H10" s="10">
+        <v>13.4</v>
+      </c>
+      <c r="I10" s="9">
+        <f>(E10/(D10*365))*100</f>
+        <v>2.4468109681443324</v>
+      </c>
+      <c r="J10" s="36">
+        <f t="shared" si="0"/>
+        <v>11.932158297306286</v>
+      </c>
+      <c r="K10" s="9">
+        <f>F10/E10</f>
+        <v>3.2272383960450424</v>
+      </c>
+      <c r="L10" s="31">
+        <f>I10*K10</f>
+        <v>7.8964423042595326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A11" s="29">
+        <v>2004</v>
+      </c>
+      <c r="B11" s="4">
+        <v>66</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3131</v>
+      </c>
+      <c r="D11" s="5">
+        <v>6917</v>
+      </c>
+      <c r="E11" s="5">
+        <v>89786</v>
+      </c>
+      <c r="F11" s="5">
+        <v>247113</v>
+      </c>
+      <c r="G11" s="4">
+        <v>424.3</v>
+      </c>
+      <c r="H11" s="10">
+        <v>15.2</v>
+      </c>
+      <c r="I11" s="9">
+        <f>(E11/(D11*365))*100</f>
+        <v>3.5562966762453434</v>
+      </c>
+      <c r="J11" s="36">
+        <f t="shared" si="0"/>
+        <v>13.551580964548068</v>
+      </c>
+      <c r="K11" s="9">
+        <f>F11/E11</f>
+        <v>2.7522442251575971</v>
+      </c>
+      <c r="L11" s="31">
+        <f>I11*K11</f>
+        <v>9.7877969901434039</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A12" s="29">
+        <v>2005</v>
+      </c>
+      <c r="B12" s="1">
+        <v>64</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3498</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7461</v>
+      </c>
+      <c r="E12" s="2">
+        <v>124254</v>
+      </c>
+      <c r="F12" s="2">
+        <v>325859</v>
+      </c>
+      <c r="G12" s="1">
+        <v>541.5</v>
+      </c>
+      <c r="H12" s="10">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="I12" s="9">
+        <f>(E12/(D12*365))*100</f>
+        <v>4.5626848654097198</v>
+      </c>
+      <c r="J12" s="36">
+        <f t="shared" si="0"/>
+        <v>15.480274442538594</v>
+      </c>
+      <c r="K12" s="9">
+        <f>F12/E12</f>
+        <v>2.6225232185684164</v>
+      </c>
+      <c r="L12" s="31">
+        <f>I12*K12</f>
+        <v>11.965746998547701</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A13" s="29">
+        <v>2006</v>
+      </c>
+      <c r="B13" s="4">
+        <v>68</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3753</v>
+      </c>
+      <c r="D13" s="5">
+        <v>8167</v>
+      </c>
+      <c r="E13" s="5">
+        <v>149102</v>
+      </c>
+      <c r="F13" s="5">
+        <v>375536</v>
+      </c>
+      <c r="G13" s="4">
+        <v>609.29999999999995</v>
+      </c>
+      <c r="H13" s="10">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="I13" s="9">
+        <f>(E13/(D13*365))*100</f>
+        <v>5.0018198865799715</v>
+      </c>
+      <c r="J13" s="36">
+        <f t="shared" si="0"/>
+        <v>16.235011990407671</v>
+      </c>
+      <c r="K13" s="9">
+        <f>F13/E13</f>
+        <v>2.5186516612788559</v>
+      </c>
+      <c r="L13" s="31">
+        <f>I13*K13</f>
+        <v>12.597841966752263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A14" s="29">
+        <v>2007</v>
+      </c>
+      <c r="B14" s="1">
+        <v>70</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3731</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8731</v>
+      </c>
+      <c r="E14" s="2">
+        <v>312850</v>
+      </c>
+      <c r="F14" s="2">
+        <v>671774</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1025.0999999999999</v>
+      </c>
+      <c r="H14" s="10">
+        <v>27.8</v>
+      </c>
+      <c r="I14" s="9">
+        <f>(E14/(D14*365))*100</f>
+        <v>9.8170116558381952</v>
+      </c>
+      <c r="J14" s="36">
+        <f t="shared" si="0"/>
+        <v>27.475207719110156</v>
+      </c>
+      <c r="K14" s="9">
+        <f>F14/E14</f>
+        <v>2.1472718555218155</v>
+      </c>
+      <c r="L14" s="31">
+        <f>I14*K14</f>
+        <v>21.079792833910972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A15" s="30">
+        <v>2008</v>
+      </c>
+      <c r="B15" s="12">
+        <v>80</v>
+      </c>
+      <c r="C15" s="13">
+        <v>4212</v>
+      </c>
+      <c r="D15" s="13">
+        <v>9331</v>
+      </c>
+      <c r="E15" s="13">
+        <v>444196</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1119360</v>
+      </c>
+      <c r="G15" s="14">
+        <v>1545.7</v>
+      </c>
+      <c r="H15" s="12">
+        <v>50.8</v>
+      </c>
+      <c r="I15" s="15">
+        <f>(E15/(D15*365))*100</f>
+        <v>13.042282096943023</v>
+      </c>
+      <c r="J15" s="36">
+        <f t="shared" si="0"/>
+        <v>36.697530864197532</v>
+      </c>
+      <c r="K15" s="15">
+        <f>F15/E15</f>
+        <v>2.5199686624823276</v>
+      </c>
+      <c r="L15" s="15">
+        <f>I15*K15</f>
+        <v>32.866142171550713</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A16" s="29">
+        <v>2009</v>
+      </c>
+      <c r="B16" s="1">
+        <v>92</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4244</v>
+      </c>
+      <c r="D16" s="2">
+        <v>9305</v>
+      </c>
+      <c r="E16" s="2">
+        <v>451840</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1041246</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1479.1</v>
+      </c>
+      <c r="H16" s="10">
+        <v>34.9</v>
+      </c>
+      <c r="I16" s="9">
+        <f>(E16/(D16*365))*100</f>
+        <v>13.30379159827166</v>
+      </c>
+      <c r="J16" s="36">
+        <f t="shared" si="0"/>
+        <v>34.851555136663521</v>
+      </c>
+      <c r="K16" s="9">
+        <f>F16/E16</f>
+        <v>2.3044573300283284</v>
+      </c>
+      <c r="L16" s="31">
+        <f>I16*K16</f>
+        <v>30.658020065806419</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A17" s="29">
+        <v>2010</v>
+      </c>
+      <c r="B17" s="4">
+        <v>87</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4590</v>
+      </c>
+      <c r="D17" s="5">
+        <v>9969</v>
+      </c>
+      <c r="E17" s="5">
+        <v>576159</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1283178</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1740.5</v>
+      </c>
+      <c r="H17" s="10">
+        <v>37.9</v>
+      </c>
+      <c r="I17" s="9">
+        <f>(E17/(D17*365))*100</f>
+        <v>15.834264301526513</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="0"/>
+        <v>37.919389978213509</v>
+      </c>
+      <c r="K17" s="9">
+        <f>F17/E17</f>
+        <v>2.2271248040905376</v>
+      </c>
+      <c r="L17" s="31">
+        <f>I17*K17</f>
+        <v>35.264882780455032</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A18" s="29">
+        <v>2011</v>
+      </c>
+      <c r="B18" s="1">
+        <v>91</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4991</v>
+      </c>
+      <c r="D18" s="2">
+        <v>10703</v>
+      </c>
+      <c r="E18" s="2">
+        <v>507372</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1245509</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1417.1</v>
+      </c>
+      <c r="H18" s="10">
+        <v>28.4</v>
+      </c>
+      <c r="I18" s="9">
+        <f>(E18/(D18*365))*100</f>
+        <v>12.987576137275555</v>
+      </c>
+      <c r="J18" s="36">
+        <f t="shared" si="0"/>
+        <v>28.393107593668603</v>
+      </c>
+      <c r="K18" s="9">
+        <f>F18/E18</f>
+        <v>2.4548240738550806</v>
+      </c>
+      <c r="L18" s="31">
+        <f>I18*K18</f>
+        <v>31.882214562809811</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A19" s="29">
+        <v>2012</v>
+      </c>
+      <c r="B19" s="4">
+        <v>98</v>
+      </c>
+      <c r="C19" s="5">
+        <v>5203</v>
+      </c>
+      <c r="D19" s="5">
+        <v>11883</v>
+      </c>
+      <c r="E19" s="5">
+        <v>575495</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1336860</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1513.7</v>
+      </c>
+      <c r="H19" s="10">
+        <v>29.1</v>
+      </c>
+      <c r="I19" s="9">
+        <f>(E19/(D19*365))*100</f>
+        <v>13.268523353841507</v>
+      </c>
+      <c r="J19" s="36">
+        <f t="shared" si="0"/>
+        <v>29.092831059004421</v>
+      </c>
+      <c r="K19" s="9">
+        <f>F19/E19</f>
+        <v>2.3229741353096029</v>
+      </c>
+      <c r="L19" s="31">
+        <f>I19*K19</f>
+        <v>30.822436564725248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A20" s="29">
+        <v>2013</v>
+      </c>
+      <c r="B20" s="1">
+        <v>113</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5890</v>
+      </c>
+      <c r="D20" s="2">
+        <v>13458</v>
+      </c>
+      <c r="E20" s="2">
+        <v>600362</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1467709</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1458.5</v>
+      </c>
+      <c r="H20" s="10">
+        <v>24.8</v>
+      </c>
+      <c r="I20" s="9">
+        <f>(E20/(D20*365))*100</f>
+        <v>12.221930429932188</v>
+      </c>
+      <c r="J20" s="36">
+        <f t="shared" si="0"/>
+        <v>24.762308998302206</v>
+      </c>
+      <c r="K20" s="9">
+        <f>F20/E20</f>
+        <v>2.4447066936281776</v>
+      </c>
+      <c r="L20" s="31">
+        <f>I20*K20</f>
+        <v>29.879035131113131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A21" s="29">
+        <v>2014</v>
+      </c>
+      <c r="B21" s="4">
+        <v>109</v>
+      </c>
+      <c r="C21" s="5">
+        <v>6666</v>
+      </c>
+      <c r="D21" s="5">
+        <v>14769</v>
+      </c>
+      <c r="E21" s="5">
+        <v>610347</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1537311</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1681.9</v>
+      </c>
+      <c r="H21" s="10">
+        <v>25.2</v>
+      </c>
+      <c r="I21" s="9">
+        <f>(E21/(D21*365))*100</f>
+        <v>11.322253108834962</v>
+      </c>
+      <c r="J21" s="36">
+        <f t="shared" si="0"/>
+        <v>25.231023102310235</v>
+      </c>
+      <c r="K21" s="9">
+        <f>F21/E21</f>
+        <v>2.5187491705537997</v>
+      </c>
+      <c r="L21" s="31">
+        <f>I21*K21</f>
+        <v>28.517915626678242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A22" s="29">
+        <v>2015</v>
+      </c>
+      <c r="B22" s="1">
+        <v>112</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6791</v>
+      </c>
+      <c r="D22" s="2">
+        <v>15059</v>
+      </c>
+      <c r="E22" s="2">
+        <v>484394</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1420264</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1530.5</v>
+      </c>
+      <c r="H22" s="10">
+        <v>22.5</v>
+      </c>
+      <c r="I22" s="9">
+        <f>(E22/(D22*365))*100</f>
+        <v>8.8127156472213866</v>
+      </c>
+      <c r="J22" s="36">
+        <f t="shared" si="0"/>
+        <v>22.537181563834487</v>
+      </c>
+      <c r="K22" s="9">
+        <f>F22/E22</f>
+        <v>2.9320429237356369</v>
+      </c>
+      <c r="L22" s="31">
+        <f>I22*K22</f>
+        <v>25.83926055232979</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="18">
+        <f>MIN(B3:B22)</f>
+        <v>57</v>
+      </c>
+      <c r="C24" s="18">
+        <f t="shared" ref="C24:L24" si="1">MIN(C3:C22)</f>
+        <v>2830</v>
+      </c>
+      <c r="D24" s="18">
+        <f t="shared" si="1"/>
+        <v>6159</v>
+      </c>
+      <c r="E24" s="18">
+        <f t="shared" si="1"/>
+        <v>45239</v>
+      </c>
+      <c r="F24" s="18">
+        <f t="shared" si="1"/>
+        <v>156676</v>
+      </c>
+      <c r="G24" s="18">
+        <f t="shared" si="1"/>
+        <v>280.8</v>
+      </c>
+      <c r="H24" s="18">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="I24" s="32">
+        <f t="shared" si="1"/>
+        <v>2.012379700493987</v>
+      </c>
+      <c r="J24" s="33">
+        <f t="shared" si="1"/>
+        <v>9.0404845393688245</v>
+      </c>
+      <c r="K24" s="32">
+        <f t="shared" si="1"/>
+        <v>2.1472718555218155</v>
+      </c>
+      <c r="L24" s="32">
+        <f t="shared" si="1"/>
+        <v>6.969464443391673</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="18">
+        <f>MAX(B3:B22)</f>
+        <v>113</v>
+      </c>
+      <c r="C25" s="18">
+        <f t="shared" ref="C25:L25" si="2">MAX(C3:C22)</f>
+        <v>6791</v>
+      </c>
+      <c r="D25" s="18">
+        <f t="shared" si="2"/>
+        <v>15059</v>
+      </c>
+      <c r="E25" s="18">
+        <f t="shared" si="2"/>
+        <v>610347</v>
+      </c>
+      <c r="F25" s="18">
+        <f t="shared" si="2"/>
+        <v>1537311</v>
+      </c>
+      <c r="G25" s="18">
+        <f t="shared" si="2"/>
+        <v>1740.5</v>
+      </c>
+      <c r="H25" s="18">
+        <f t="shared" si="2"/>
+        <v>50.8</v>
+      </c>
+      <c r="I25" s="32">
+        <f t="shared" si="2"/>
+        <v>15.834264301526513</v>
+      </c>
+      <c r="J25" s="33">
+        <f t="shared" si="2"/>
+        <v>37.919389978213509</v>
+      </c>
+      <c r="K25" s="32">
+        <f t="shared" si="2"/>
+        <v>3.4632949446274233</v>
+      </c>
+      <c r="L25" s="32">
+        <f t="shared" si="2"/>
+        <v>35.264882780455032</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A3:L22">
+    <sortCondition ref="A3:A22"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed typo in sheet 2
</commit_message>
<xml_diff>
--- a/WestBank-Hotels.xlsx
+++ b/WestBank-Hotels.xlsx
@@ -275,13 +275,13 @@
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,7 +334,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>متوسط الإشغال السنوي لكل 200 سرير</c:v>
+            <c:v>متوسط الإشغال السنوي لكل 100 سرير</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="38100">
@@ -676,11 +676,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="59704832"/>
-        <c:axId val="1208256"/>
+        <c:axId val="1090543616"/>
+        <c:axId val="618148928"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="59704832"/>
+        <c:axId val="1090543616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -703,14 +703,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1208256"/>
+        <c:crossAx val="618148928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1208256"/>
+        <c:axId val="618148928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,7 +732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59704832"/>
+        <c:crossAx val="1090543616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1097,7 +1097,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1117,25 +1117,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
       <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2137,7 +2137,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2148,20 +2148,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -2227,19 +2227,19 @@
         <v>38.299999999999997</v>
       </c>
       <c r="I3" s="9">
-        <f>(E3/(D3*365))*100</f>
+        <f t="shared" ref="I3:I22" si="0">(E3/(D3*365))*100</f>
         <v>9.5854785506879363</v>
       </c>
-      <c r="J3" s="36">
+      <c r="J3" s="34">
         <f>(G3/C3)*100</f>
         <v>36.49707803368856</v>
       </c>
       <c r="K3" s="9">
-        <f>F3/E3</f>
+        <f t="shared" ref="K3:K22" si="1">F3/E3</f>
         <v>3.1967741646591019</v>
       </c>
       <c r="L3" s="31">
-        <f>I3*K3</f>
+        <f t="shared" ref="L3:L22" si="2">I3*K3</f>
         <v>30.642610186733165</v>
       </c>
     </row>
@@ -2269,19 +2269,19 @@
         <v>31.7</v>
       </c>
       <c r="I4" s="9">
-        <f>(E4/(D4*365))*100</f>
+        <f t="shared" si="0"/>
         <v>8.501853905122978</v>
       </c>
-      <c r="J4" s="36">
-        <f t="shared" ref="J4:J22" si="0">(G4/C4)*100</f>
+      <c r="J4" s="34">
+        <f t="shared" ref="J4:J22" si="3">(G4/C4)*100</f>
         <v>30.044359949302919</v>
       </c>
       <c r="K4" s="9">
-        <f>F4/E4</f>
+        <f t="shared" si="1"/>
         <v>2.8861372485778256</v>
       </c>
       <c r="L4" s="31">
-        <f>I4*K4</f>
+        <f t="shared" si="2"/>
         <v>24.537517237542275</v>
       </c>
     </row>
@@ -2311,19 +2311,19 @@
         <v>27.5</v>
       </c>
       <c r="I5" s="9">
-        <f>(E5/(D5*365))*100</f>
+        <f t="shared" si="0"/>
         <v>7.4061613862483267</v>
       </c>
-      <c r="J5" s="36">
-        <f t="shared" si="0"/>
+      <c r="J5" s="34">
+        <f t="shared" si="3"/>
         <v>25.808314087759815</v>
       </c>
       <c r="K5" s="9">
-        <f>F5/E5</f>
+        <f t="shared" si="1"/>
         <v>2.8137521339010654</v>
       </c>
       <c r="L5" s="31">
-        <f>I5*K5</f>
+        <f t="shared" si="2"/>
         <v>20.8391024045719</v>
       </c>
     </row>
@@ -2353,19 +2353,19 @@
         <v>35.5</v>
       </c>
       <c r="I6" s="9">
-        <f>(E6/(D6*365))*100</f>
+        <f t="shared" si="0"/>
         <v>10.793556075568839</v>
       </c>
-      <c r="J6" s="36">
-        <f t="shared" si="0"/>
+      <c r="J6" s="34">
+        <f t="shared" si="3"/>
         <v>33.717032967032964</v>
       </c>
       <c r="K6" s="9">
-        <f>F6/E6</f>
+        <f t="shared" si="1"/>
         <v>2.7345860359868088</v>
       </c>
       <c r="L6" s="31">
-        <f>I6*K6</f>
+        <f t="shared" si="2"/>
         <v>29.515907722891129</v>
       </c>
     </row>
@@ -2395,19 +2395,19 @@
         <v>35.1</v>
       </c>
       <c r="I7" s="9">
-        <f>(E7/(D7*365))*100</f>
+        <f t="shared" si="0"/>
         <v>9.4924952193103778</v>
       </c>
-      <c r="J7" s="36">
-        <f t="shared" si="0"/>
+      <c r="J7" s="34">
+        <f t="shared" si="3"/>
         <v>32.219878105954052</v>
       </c>
       <c r="K7" s="9">
-        <f>F7/E7</f>
+        <f t="shared" si="1"/>
         <v>3.0675147049973237</v>
       </c>
       <c r="L7" s="31">
-        <f>I7*K7</f>
+        <f t="shared" si="2"/>
         <v>29.11836867235138</v>
       </c>
     </row>
@@ -2437,19 +2437,19 @@
         <v>8.4</v>
       </c>
       <c r="I8" s="9">
-        <f>(E8/(D8*365))*100</f>
+        <f t="shared" si="0"/>
         <v>2.3774915921581496</v>
       </c>
-      <c r="J8" s="36">
-        <f t="shared" si="0"/>
+      <c r="J8" s="34">
+        <f t="shared" si="3"/>
         <v>9.0404845393688245</v>
       </c>
       <c r="K8" s="9">
-        <f>F8/E8</f>
+        <f t="shared" si="1"/>
         <v>3.0599468672370964</v>
       </c>
       <c r="L8" s="31">
-        <f>I8*K8</f>
+        <f t="shared" si="2"/>
         <v>7.2749979493068668</v>
       </c>
     </row>
@@ -2479,19 +2479,19 @@
         <v>11.3</v>
       </c>
       <c r="I9" s="9">
-        <f>(E9/(D9*365))*100</f>
+        <f t="shared" si="0"/>
         <v>2.012379700493987</v>
       </c>
-      <c r="J9" s="36">
-        <f t="shared" si="0"/>
+      <c r="J9" s="34">
+        <f t="shared" si="3"/>
         <v>9.9222614840989412</v>
       </c>
       <c r="K9" s="9">
-        <f>F9/E9</f>
+        <f t="shared" si="1"/>
         <v>3.4632949446274233</v>
       </c>
       <c r="L9" s="31">
-        <f>I9*K9</f>
+        <f t="shared" si="2"/>
         <v>6.969464443391673</v>
       </c>
     </row>
@@ -2521,19 +2521,19 @@
         <v>13.4</v>
       </c>
       <c r="I10" s="9">
-        <f>(E10/(D10*365))*100</f>
+        <f t="shared" si="0"/>
         <v>2.4468109681443324</v>
       </c>
-      <c r="J10" s="36">
-        <f t="shared" si="0"/>
+      <c r="J10" s="34">
+        <f t="shared" si="3"/>
         <v>11.932158297306286</v>
       </c>
       <c r="K10" s="9">
-        <f>F10/E10</f>
+        <f t="shared" si="1"/>
         <v>3.2272383960450424</v>
       </c>
       <c r="L10" s="31">
-        <f>I10*K10</f>
+        <f t="shared" si="2"/>
         <v>7.8964423042595326</v>
       </c>
     </row>
@@ -2563,19 +2563,19 @@
         <v>15.2</v>
       </c>
       <c r="I11" s="9">
-        <f>(E11/(D11*365))*100</f>
+        <f t="shared" si="0"/>
         <v>3.5562966762453434</v>
       </c>
-      <c r="J11" s="36">
-        <f t="shared" si="0"/>
+      <c r="J11" s="34">
+        <f t="shared" si="3"/>
         <v>13.551580964548068</v>
       </c>
       <c r="K11" s="9">
-        <f>F11/E11</f>
+        <f t="shared" si="1"/>
         <v>2.7522442251575971</v>
       </c>
       <c r="L11" s="31">
-        <f>I11*K11</f>
+        <f t="shared" si="2"/>
         <v>9.7877969901434039</v>
       </c>
     </row>
@@ -2605,19 +2605,19 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I12" s="9">
-        <f>(E12/(D12*365))*100</f>
+        <f t="shared" si="0"/>
         <v>4.5626848654097198</v>
       </c>
-      <c r="J12" s="36">
-        <f t="shared" si="0"/>
+      <c r="J12" s="34">
+        <f t="shared" si="3"/>
         <v>15.480274442538594</v>
       </c>
       <c r="K12" s="9">
-        <f>F12/E12</f>
+        <f t="shared" si="1"/>
         <v>2.6225232185684164</v>
       </c>
       <c r="L12" s="31">
-        <f>I12*K12</f>
+        <f t="shared" si="2"/>
         <v>11.965746998547701</v>
       </c>
     </row>
@@ -2647,19 +2647,19 @@
         <v>17.600000000000001</v>
       </c>
       <c r="I13" s="9">
-        <f>(E13/(D13*365))*100</f>
+        <f t="shared" si="0"/>
         <v>5.0018198865799715</v>
       </c>
-      <c r="J13" s="36">
-        <f t="shared" si="0"/>
+      <c r="J13" s="34">
+        <f t="shared" si="3"/>
         <v>16.235011990407671</v>
       </c>
       <c r="K13" s="9">
-        <f>F13/E13</f>
+        <f t="shared" si="1"/>
         <v>2.5186516612788559</v>
       </c>
       <c r="L13" s="31">
-        <f>I13*K13</f>
+        <f t="shared" si="2"/>
         <v>12.597841966752263</v>
       </c>
     </row>
@@ -2689,19 +2689,19 @@
         <v>27.8</v>
       </c>
       <c r="I14" s="9">
-        <f>(E14/(D14*365))*100</f>
+        <f t="shared" si="0"/>
         <v>9.8170116558381952</v>
       </c>
-      <c r="J14" s="36">
-        <f t="shared" si="0"/>
+      <c r="J14" s="34">
+        <f t="shared" si="3"/>
         <v>27.475207719110156</v>
       </c>
       <c r="K14" s="9">
-        <f>F14/E14</f>
+        <f t="shared" si="1"/>
         <v>2.1472718555218155</v>
       </c>
       <c r="L14" s="31">
-        <f>I14*K14</f>
+        <f t="shared" si="2"/>
         <v>21.079792833910972</v>
       </c>
     </row>
@@ -2731,19 +2731,19 @@
         <v>50.8</v>
       </c>
       <c r="I15" s="15">
-        <f>(E15/(D15*365))*100</f>
+        <f t="shared" si="0"/>
         <v>13.042282096943023</v>
       </c>
-      <c r="J15" s="36">
-        <f t="shared" si="0"/>
+      <c r="J15" s="34">
+        <f t="shared" si="3"/>
         <v>36.697530864197532</v>
       </c>
       <c r="K15" s="15">
-        <f>F15/E15</f>
+        <f t="shared" si="1"/>
         <v>2.5199686624823276</v>
       </c>
       <c r="L15" s="15">
-        <f>I15*K15</f>
+        <f t="shared" si="2"/>
         <v>32.866142171550713</v>
       </c>
     </row>
@@ -2773,19 +2773,19 @@
         <v>34.9</v>
       </c>
       <c r="I16" s="9">
-        <f>(E16/(D16*365))*100</f>
+        <f t="shared" si="0"/>
         <v>13.30379159827166</v>
       </c>
-      <c r="J16" s="36">
-        <f t="shared" si="0"/>
+      <c r="J16" s="34">
+        <f t="shared" si="3"/>
         <v>34.851555136663521</v>
       </c>
       <c r="K16" s="9">
-        <f>F16/E16</f>
+        <f t="shared" si="1"/>
         <v>2.3044573300283284</v>
       </c>
       <c r="L16" s="31">
-        <f>I16*K16</f>
+        <f t="shared" si="2"/>
         <v>30.658020065806419</v>
       </c>
     </row>
@@ -2815,19 +2815,19 @@
         <v>37.9</v>
       </c>
       <c r="I17" s="9">
-        <f>(E17/(D17*365))*100</f>
+        <f t="shared" si="0"/>
         <v>15.834264301526513</v>
       </c>
-      <c r="J17" s="36">
-        <f t="shared" si="0"/>
+      <c r="J17" s="34">
+        <f t="shared" si="3"/>
         <v>37.919389978213509</v>
       </c>
       <c r="K17" s="9">
-        <f>F17/E17</f>
+        <f t="shared" si="1"/>
         <v>2.2271248040905376</v>
       </c>
       <c r="L17" s="31">
-        <f>I17*K17</f>
+        <f t="shared" si="2"/>
         <v>35.264882780455032</v>
       </c>
     </row>
@@ -2857,19 +2857,19 @@
         <v>28.4</v>
       </c>
       <c r="I18" s="9">
-        <f>(E18/(D18*365))*100</f>
+        <f t="shared" si="0"/>
         <v>12.987576137275555</v>
       </c>
-      <c r="J18" s="36">
-        <f t="shared" si="0"/>
+      <c r="J18" s="34">
+        <f t="shared" si="3"/>
         <v>28.393107593668603</v>
       </c>
       <c r="K18" s="9">
-        <f>F18/E18</f>
+        <f t="shared" si="1"/>
         <v>2.4548240738550806</v>
       </c>
       <c r="L18" s="31">
-        <f>I18*K18</f>
+        <f t="shared" si="2"/>
         <v>31.882214562809811</v>
       </c>
     </row>
@@ -2899,19 +2899,19 @@
         <v>29.1</v>
       </c>
       <c r="I19" s="9">
-        <f>(E19/(D19*365))*100</f>
+        <f t="shared" si="0"/>
         <v>13.268523353841507</v>
       </c>
-      <c r="J19" s="36">
-        <f t="shared" si="0"/>
+      <c r="J19" s="34">
+        <f t="shared" si="3"/>
         <v>29.092831059004421</v>
       </c>
       <c r="K19" s="9">
-        <f>F19/E19</f>
+        <f t="shared" si="1"/>
         <v>2.3229741353096029</v>
       </c>
       <c r="L19" s="31">
-        <f>I19*K19</f>
+        <f t="shared" si="2"/>
         <v>30.822436564725248</v>
       </c>
     </row>
@@ -2941,19 +2941,19 @@
         <v>24.8</v>
       </c>
       <c r="I20" s="9">
-        <f>(E20/(D20*365))*100</f>
+        <f t="shared" si="0"/>
         <v>12.221930429932188</v>
       </c>
-      <c r="J20" s="36">
-        <f t="shared" si="0"/>
+      <c r="J20" s="34">
+        <f t="shared" si="3"/>
         <v>24.762308998302206</v>
       </c>
       <c r="K20" s="9">
-        <f>F20/E20</f>
+        <f t="shared" si="1"/>
         <v>2.4447066936281776</v>
       </c>
       <c r="L20" s="31">
-        <f>I20*K20</f>
+        <f t="shared" si="2"/>
         <v>29.879035131113131</v>
       </c>
     </row>
@@ -2983,19 +2983,19 @@
         <v>25.2</v>
       </c>
       <c r="I21" s="9">
-        <f>(E21/(D21*365))*100</f>
+        <f t="shared" si="0"/>
         <v>11.322253108834962</v>
       </c>
-      <c r="J21" s="36">
-        <f t="shared" si="0"/>
+      <c r="J21" s="34">
+        <f t="shared" si="3"/>
         <v>25.231023102310235</v>
       </c>
       <c r="K21" s="9">
-        <f>F21/E21</f>
+        <f t="shared" si="1"/>
         <v>2.5187491705537997</v>
       </c>
       <c r="L21" s="31">
-        <f>I21*K21</f>
+        <f t="shared" si="2"/>
         <v>28.517915626678242</v>
       </c>
     </row>
@@ -3025,19 +3025,19 @@
         <v>22.5</v>
       </c>
       <c r="I22" s="9">
-        <f>(E22/(D22*365))*100</f>
+        <f t="shared" si="0"/>
         <v>8.8127156472213866</v>
       </c>
-      <c r="J22" s="36">
-        <f t="shared" si="0"/>
+      <c r="J22" s="34">
+        <f t="shared" si="3"/>
         <v>22.537181563834487</v>
       </c>
       <c r="K22" s="9">
-        <f>F22/E22</f>
+        <f t="shared" si="1"/>
         <v>2.9320429237356369</v>
       </c>
       <c r="L22" s="31">
-        <f>I22*K22</f>
+        <f t="shared" si="2"/>
         <v>25.83926055232979</v>
       </c>
     </row>
@@ -3064,43 +3064,43 @@
         <v>57</v>
       </c>
       <c r="C24" s="18">
-        <f t="shared" ref="C24:L24" si="1">MIN(C3:C22)</f>
+        <f t="shared" ref="C24:L24" si="4">MIN(C3:C22)</f>
         <v>2830</v>
       </c>
       <c r="D24" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6159</v>
       </c>
       <c r="E24" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45239</v>
       </c>
       <c r="F24" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>156676</v>
       </c>
       <c r="G24" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>280.8</v>
       </c>
       <c r="H24" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.4</v>
       </c>
       <c r="I24" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.012379700493987</v>
       </c>
       <c r="J24" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.0404845393688245</v>
       </c>
       <c r="K24" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.1472718555218155</v>
       </c>
       <c r="L24" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.969464443391673</v>
       </c>
     </row>
@@ -3113,43 +3113,43 @@
         <v>113</v>
       </c>
       <c r="C25" s="18">
-        <f t="shared" ref="C25:L25" si="2">MAX(C3:C22)</f>
+        <f t="shared" ref="C25:L25" si="5">MAX(C3:C22)</f>
         <v>6791</v>
       </c>
       <c r="D25" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>15059</v>
       </c>
       <c r="E25" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>610347</v>
       </c>
       <c r="F25" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1537311</v>
       </c>
       <c r="G25" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1740.5</v>
       </c>
       <c r="H25" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>50.8</v>
       </c>
       <c r="I25" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>15.834264301526513</v>
       </c>
       <c r="J25" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>37.919389978213509</v>
       </c>
       <c r="K25" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.4632949446274233</v>
       </c>
       <c r="L25" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>35.264882780455032</v>
       </c>
     </row>

</xml_diff>